<commit_message>
performed lstm and bilstm
</commit_message>
<xml_diff>
--- a/Results_ST1.xlsx
+++ b/Results_ST1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitanshjain/Documents/Projects/CASE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{679DA22C-3ED6-C846-A884-1044460920C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD02C3A-685C-E743-AFF9-5329561FB150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C5EB9B45-C453-ED44-A410-DAC4C6713FD6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
   <si>
     <t>Dataset</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>MNB</t>
+  </si>
+  <si>
+    <t>Embeddings</t>
+  </si>
+  <si>
+    <t>FastText</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>MinMax</t>
   </si>
 </sst>
 </file>
@@ -411,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58CF967-29B9-EC40-8123-04EA241913C3}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,7 +439,7 @@
     <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -446,69 +458,219 @@
       <c r="F1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.46</v>
+      </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.46</v>
+      </c>
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.44</v>
+      </c>
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5">
+        <v>0.65</v>
+      </c>
+      <c r="C5">
+        <v>0.09</v>
+      </c>
+      <c r="D5">
+        <v>0.16</v>
+      </c>
+      <c r="E5">
+        <v>0.48</v>
+      </c>
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="B6">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="C6">
+        <v>0.9</v>
+      </c>
+      <c r="D6">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="E6">
+        <v>0.57999999999999996</v>
+      </c>
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.46</v>
+      </c>
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C8">
+        <v>0.76</v>
+      </c>
+      <c r="D8">
+        <v>0.65</v>
+      </c>
+      <c r="E8">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="F8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.45</v>
+      </c>
       <c r="F9">
         <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>